<commit_message>
Added third driven oscillation dataset
</commit_message>
<xml_diff>
--- a/Cavendish_Experiment/Data/20171024_cavendish_by_hand_data.xlsx
+++ b/Cavendish_Experiment/Data/20171024_cavendish_by_hand_data.xlsx
@@ -171,10 +171,16 @@
     <numFmt numFmtId="165" formatCode="0.000E+00"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1030,10 +1036,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1743,6 +1752,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="79" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>